<commit_message>
feat: add transformaciones y notas
</commit_message>
<xml_diff>
--- a/codebook.xlsx
+++ b/codebook.xlsx
@@ -519,8 +519,16 @@
           <t>{'count': 30.0, 'mean': 116596421.7, 'std': 114813944.03975926, 'min': 4772877.0, '25%': 15739203.0, '50%': 70778086.0, '75%': 226772072.25, 'max': 320462039.0}</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>ID codificado, entero positivo</t>
+        </is>
+      </c>
       <c r="J2" t="inlineStr"/>
     </row>
     <row r="3">
@@ -553,8 +561,16 @@
           <t>{'unique': 30, 'top': 'MDEwOlJlcG9zaXRvcnk0MTY0NTExOQ==', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>ID codificado, entero positivo</t>
+        </is>
+      </c>
       <c r="J3" t="inlineStr"/>
     </row>
     <row r="4">
@@ -587,7 +603,11 @@
           <t>{'unique': 30, 'top': '2018', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
     </row>
@@ -621,7 +641,11 @@
           <t>{'unique': 30, 'top': 'jtleek/2018', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
     </row>
@@ -655,7 +679,11 @@
           <t>{'count': 30, 'unique': 1, 'top': False, 'freq': 30}</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr"/>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr"/>
     </row>
@@ -689,7 +717,11 @@
           <t>{'unique': 1, 'top': "{'login': 'jtleek', 'id': 1571674, 'node_id': 'MDQ6VXNlcjE1NzE2NzQ=', 'avatar_url': 'https://avatars.githubusercontent.com/u/1571674?v=4', 'gravatar_id': '', 'url': 'https://api.github.com/users/jtleek', 'html_url': 'https://github.com/jtleek', 'followers_url': 'https://api.github.com/users/jtleek/followers', 'following_url': 'https://api.github.com/users/jtleek/following{/other_user}', 'gists_url': 'https://api.github.com/users/jtleek/gists{/gist_id}', 'starred_url': 'https://api.github.com/users/jtleek/starred{/owner}{/repo}', 'subscriptions_url': 'https://api.github.com/users/jtleek/subscriptions', 'organizations_url': 'https://api.github.com/users/jtleek/orgs', 'repos_url': 'https://api.github.com/users/jtleek/repos', 'events_url': 'https://api.github.com/users/jtleek/events{/privacy}', 'received_events_url': 'https://api.github.com/users/jtleek/received_events', 'type': 'User', 'site_admin': False}", 'freq': 30}</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr"/>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
     </row>
@@ -723,7 +755,11 @@
           <t>{'unique': 30, 'top': 'https://github.com/jtleek/2018', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr"/>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
     </row>
@@ -757,7 +793,11 @@
           <t>{'unique': 23, 'top': 'A career planning guide.', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr"/>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
     </row>
@@ -791,7 +831,11 @@
           <t>{'count': 30, 'unique': 2, 'top': False, 'freq': 20}</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr"/>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
     </row>
@@ -825,7 +869,11 @@
           <t>{'unique': 30, 'top': 'https://api.github.com/repos/jtleek/2018', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr"/>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr"/>
     </row>
@@ -859,7 +907,11 @@
           <t>{'unique': 30, 'top': 'https://api.github.com/repos/jtleek/2018/forks', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr"/>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr"/>
     </row>
@@ -893,7 +945,11 @@
           <t>{'unique': 30, 'top': 'https://api.github.com/repos/jtleek/2018/keys{/key_id}', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr"/>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
     </row>
@@ -927,7 +983,11 @@
           <t>{'unique': 30, 'top': 'https://api.github.com/repos/jtleek/2018/collaborators{/collaborator}', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr"/>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr"/>
     </row>
@@ -961,7 +1021,11 @@
           <t>{'unique': 30, 'top': 'https://api.github.com/repos/jtleek/2018/teams', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr"/>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr"/>
     </row>
@@ -995,7 +1059,11 @@
           <t>{'unique': 30, 'top': 'https://api.github.com/repos/jtleek/2018/hooks', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr"/>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr"/>
     </row>
@@ -1029,7 +1097,11 @@
           <t>{'unique': 30, 'top': 'https://api.github.com/repos/jtleek/2018/issues/events{/number}', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr"/>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr"/>
     </row>
@@ -1063,7 +1135,11 @@
           <t>{'unique': 30, 'top': 'https://api.github.com/repos/jtleek/2018/events', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H18" t="inlineStr"/>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr"/>
     </row>
@@ -1097,7 +1173,11 @@
           <t>{'unique': 30, 'top': 'https://api.github.com/repos/jtleek/2018/assignees{/user}', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H19" t="inlineStr"/>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr"/>
     </row>
@@ -1131,7 +1211,11 @@
           <t>{'unique': 30, 'top': 'https://api.github.com/repos/jtleek/2018/branches{/branch}', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr"/>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr"/>
     </row>
@@ -1165,7 +1249,11 @@
           <t>{'unique': 30, 'top': 'https://api.github.com/repos/jtleek/2018/tags', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H21" t="inlineStr"/>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr"/>
     </row>
@@ -1199,7 +1287,11 @@
           <t>{'unique': 30, 'top': 'https://api.github.com/repos/jtleek/2018/git/blobs{/sha}', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H22" t="inlineStr"/>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr"/>
     </row>
@@ -1233,7 +1325,11 @@
           <t>{'unique': 30, 'top': 'https://api.github.com/repos/jtleek/2018/git/tags{/sha}', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H23" t="inlineStr"/>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I23" t="inlineStr"/>
       <c r="J23" t="inlineStr"/>
     </row>
@@ -1267,7 +1363,11 @@
           <t>{'unique': 30, 'top': 'https://api.github.com/repos/jtleek/2018/git/refs{/sha}', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H24" t="inlineStr"/>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I24" t="inlineStr"/>
       <c r="J24" t="inlineStr"/>
     </row>
@@ -1301,7 +1401,11 @@
           <t>{'unique': 30, 'top': 'https://api.github.com/repos/jtleek/2018/git/trees{/sha}', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H25" t="inlineStr"/>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I25" t="inlineStr"/>
       <c r="J25" t="inlineStr"/>
     </row>
@@ -1335,7 +1439,11 @@
           <t>{'unique': 30, 'top': 'https://api.github.com/repos/jtleek/2018/statuses/{sha}', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H26" t="inlineStr"/>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I26" t="inlineStr"/>
       <c r="J26" t="inlineStr"/>
     </row>
@@ -1369,7 +1477,11 @@
           <t>{'unique': 30, 'top': 'https://api.github.com/repos/jtleek/2018/languages', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H27" t="inlineStr"/>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I27" t="inlineStr"/>
       <c r="J27" t="inlineStr"/>
     </row>
@@ -1403,7 +1515,11 @@
           <t>{'unique': 30, 'top': 'https://api.github.com/repos/jtleek/2018/stargazers', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H28" t="inlineStr"/>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I28" t="inlineStr"/>
       <c r="J28" t="inlineStr"/>
     </row>
@@ -1437,7 +1553,11 @@
           <t>{'unique': 30, 'top': 'https://api.github.com/repos/jtleek/2018/contributors', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H29" t="inlineStr"/>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I29" t="inlineStr"/>
       <c r="J29" t="inlineStr"/>
     </row>
@@ -1471,7 +1591,11 @@
           <t>{'unique': 30, 'top': 'https://api.github.com/repos/jtleek/2018/subscribers', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H30" t="inlineStr"/>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I30" t="inlineStr"/>
       <c r="J30" t="inlineStr"/>
     </row>
@@ -1505,7 +1629,11 @@
           <t>{'unique': 30, 'top': 'https://api.github.com/repos/jtleek/2018/subscription', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H31" t="inlineStr"/>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I31" t="inlineStr"/>
       <c r="J31" t="inlineStr"/>
     </row>
@@ -1539,7 +1667,11 @@
           <t>{'unique': 30, 'top': 'https://api.github.com/repos/jtleek/2018/commits{/sha}', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H32" t="inlineStr"/>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I32" t="inlineStr"/>
       <c r="J32" t="inlineStr"/>
     </row>
@@ -1573,7 +1705,11 @@
           <t>{'unique': 30, 'top': 'https://api.github.com/repos/jtleek/2018/git/commits{/sha}', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H33" t="inlineStr"/>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I33" t="inlineStr"/>
       <c r="J33" t="inlineStr"/>
     </row>
@@ -1607,7 +1743,11 @@
           <t>{'unique': 30, 'top': 'https://api.github.com/repos/jtleek/2018/comments{/number}', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H34" t="inlineStr"/>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I34" t="inlineStr"/>
       <c r="J34" t="inlineStr"/>
     </row>
@@ -1641,7 +1781,11 @@
           <t>{'unique': 30, 'top': 'https://api.github.com/repos/jtleek/2018/issues/comments{/number}', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H35" t="inlineStr"/>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I35" t="inlineStr"/>
       <c r="J35" t="inlineStr"/>
     </row>
@@ -1675,7 +1819,11 @@
           <t>{'unique': 30, 'top': 'https://api.github.com/repos/jtleek/2018/contents/{+path}', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H36" t="inlineStr"/>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I36" t="inlineStr"/>
       <c r="J36" t="inlineStr"/>
     </row>
@@ -1709,7 +1857,11 @@
           <t>{'unique': 30, 'top': 'https://api.github.com/repos/jtleek/2018/compare/{base}...{head}', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H37" t="inlineStr"/>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I37" t="inlineStr"/>
       <c r="J37" t="inlineStr"/>
     </row>
@@ -1743,7 +1895,11 @@
           <t>{'unique': 30, 'top': 'https://api.github.com/repos/jtleek/2018/merges', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H38" t="inlineStr"/>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I38" t="inlineStr"/>
       <c r="J38" t="inlineStr"/>
     </row>
@@ -1777,7 +1933,11 @@
           <t>{'unique': 30, 'top': 'https://api.github.com/repos/jtleek/2018/{archive_format}{/ref}', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H39" t="inlineStr"/>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I39" t="inlineStr"/>
       <c r="J39" t="inlineStr"/>
     </row>
@@ -1811,7 +1971,11 @@
           <t>{'unique': 30, 'top': 'https://api.github.com/repos/jtleek/2018/downloads', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H40" t="inlineStr"/>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I40" t="inlineStr"/>
       <c r="J40" t="inlineStr"/>
     </row>
@@ -1845,7 +2009,11 @@
           <t>{'unique': 30, 'top': 'https://api.github.com/repos/jtleek/2018/issues{/number}', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H41" t="inlineStr"/>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I41" t="inlineStr"/>
       <c r="J41" t="inlineStr"/>
     </row>
@@ -1879,7 +2047,11 @@
           <t>{'unique': 30, 'top': 'https://api.github.com/repos/jtleek/2018/pulls{/number}', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H42" t="inlineStr"/>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I42" t="inlineStr"/>
       <c r="J42" t="inlineStr"/>
     </row>
@@ -1913,7 +2085,11 @@
           <t>{'unique': 30, 'top': 'https://api.github.com/repos/jtleek/2018/milestones{/number}', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H43" t="inlineStr"/>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I43" t="inlineStr"/>
       <c r="J43" t="inlineStr"/>
     </row>
@@ -1947,7 +2123,11 @@
           <t>{'unique': 30, 'top': 'https://api.github.com/repos/jtleek/2018/notifications{?since,all,participating}', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H44" t="inlineStr"/>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I44" t="inlineStr"/>
       <c r="J44" t="inlineStr"/>
     </row>
@@ -1981,7 +2161,11 @@
           <t>{'unique': 30, 'top': 'https://api.github.com/repos/jtleek/2018/labels{/name}', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H45" t="inlineStr"/>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I45" t="inlineStr"/>
       <c r="J45" t="inlineStr"/>
     </row>
@@ -2015,7 +2199,11 @@
           <t>{'unique': 30, 'top': 'https://api.github.com/repos/jtleek/2018/releases{/id}', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H46" t="inlineStr"/>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I46" t="inlineStr"/>
       <c r="J46" t="inlineStr"/>
     </row>
@@ -2049,7 +2237,11 @@
           <t>{'unique': 30, 'top': 'https://api.github.com/repos/jtleek/2018/deployments', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H47" t="inlineStr"/>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I47" t="inlineStr"/>
       <c r="J47" t="inlineStr"/>
     </row>
@@ -2087,8 +2279,16 @@
           <t>{'unique': 30, 'top': '2012-06-24T14:36:20Z', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H48" t="inlineStr"/>
-      <c r="I48" t="inlineStr"/>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>Fecha en formato ISO 8601</t>
+        </is>
+      </c>
       <c r="J48" t="inlineStr"/>
     </row>
     <row r="49">
@@ -2125,8 +2325,16 @@
           <t>{'unique': 30, 'top': '2013-08-08T13:20:42Z', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H49" t="inlineStr"/>
-      <c r="I49" t="inlineStr"/>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>Fecha en formato ISO 8601</t>
+        </is>
+      </c>
       <c r="J49" t="inlineStr"/>
     </row>
     <row r="50">
@@ -2163,8 +2371,16 @@
           <t>{'unique': 30, 'top': '2012-06-24T14:38:18Z', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H50" t="inlineStr"/>
-      <c r="I50" t="inlineStr"/>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>Fecha en formato ISO 8601</t>
+        </is>
+      </c>
       <c r="J50" t="inlineStr"/>
     </row>
     <row r="51">
@@ -2197,7 +2413,11 @@
           <t>{'unique': 30, 'top': 'git://github.com/jtleek/2018.git', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H51" t="inlineStr"/>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I51" t="inlineStr"/>
       <c r="J51" t="inlineStr"/>
     </row>
@@ -2231,7 +2451,11 @@
           <t>{'unique': 30, 'top': 'git@github.com:jtleek/2018.git', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H52" t="inlineStr"/>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I52" t="inlineStr"/>
       <c r="J52" t="inlineStr"/>
     </row>
@@ -2265,7 +2489,11 @@
           <t>{'unique': 30, 'top': 'https://github.com/jtleek/2018.git', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H53" t="inlineStr"/>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I53" t="inlineStr"/>
       <c r="J53" t="inlineStr"/>
     </row>
@@ -2299,7 +2527,11 @@
           <t>{'unique': 30, 'top': 'https://github.com/jtleek/2018', 'freq': 1}</t>
         </is>
       </c>
-      <c r="H54" t="inlineStr"/>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I54" t="inlineStr"/>
       <c r="J54" t="inlineStr"/>
     </row>
@@ -2333,7 +2565,11 @@
           <t>{'unique': 3, 'top': '', 'freq': 2}</t>
         </is>
       </c>
-      <c r="H55" t="inlineStr"/>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I55" t="inlineStr"/>
       <c r="J55" t="inlineStr"/>
     </row>
@@ -2371,8 +2607,16 @@
           <t>{'count': 30.0, 'mean': 42662.76666666667, 'std': 84113.27974889634, 'min': 0.0, '25%': 101.5, '50%': 489.0, '75%': 58141.25, 'max': 374812.0}</t>
         </is>
       </c>
-      <c r="H56" t="inlineStr"/>
-      <c r="I56" t="inlineStr"/>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>Tamaño en KB</t>
+        </is>
+      </c>
       <c r="J56" t="inlineStr"/>
     </row>
     <row r="57">
@@ -2409,8 +2653,16 @@
           <t>{'count': 30.0, 'mean': 233.76666666666668, 'std': 1066.5860032359558, 'min': 0.0, '25%': 0.25, '50%': 3.5, '75%': 9.25, 'max': 5836.0}</t>
         </is>
       </c>
-      <c r="H57" t="inlineStr"/>
-      <c r="I57" t="inlineStr"/>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>ID codificado, entero positivo</t>
+        </is>
+      </c>
       <c r="J57" t="inlineStr"/>
     </row>
     <row r="58">
@@ -2447,8 +2699,16 @@
           <t>{'count': 30.0, 'mean': 233.76666666666668, 'std': 1066.5860032359558, 'min': 0.0, '25%': 0.25, '50%': 3.5, '75%': 9.25, 'max': 5836.0}</t>
         </is>
       </c>
-      <c r="H58" t="inlineStr"/>
-      <c r="I58" t="inlineStr"/>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>ID codificado, entero positivo</t>
+        </is>
+      </c>
       <c r="J58" t="inlineStr"/>
     </row>
     <row r="59">
@@ -2481,8 +2741,16 @@
           <t>{'unique': 6, 'top': 'HTML', 'freq': 9}</t>
         </is>
       </c>
-      <c r="H59" t="inlineStr"/>
-      <c r="I59" t="inlineStr"/>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>Lenguaje de programación principal</t>
+        </is>
+      </c>
       <c r="J59" t="inlineStr"/>
     </row>
     <row r="60">
@@ -2515,8 +2783,16 @@
           <t>{'count': 30, 'unique': 2, 'top': True, 'freq': 20}</t>
         </is>
       </c>
-      <c r="H60" t="inlineStr"/>
-      <c r="I60" t="inlineStr"/>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>Booleano (True/False)</t>
+        </is>
+      </c>
       <c r="J60" t="inlineStr"/>
     </row>
     <row r="61">
@@ -2549,8 +2825,16 @@
           <t>{'count': 30, 'unique': 1, 'top': True, 'freq': 30}</t>
         </is>
       </c>
-      <c r="H61" t="inlineStr"/>
-      <c r="I61" t="inlineStr"/>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>Booleano (True/False)</t>
+        </is>
+      </c>
       <c r="J61" t="inlineStr"/>
     </row>
     <row r="62">
@@ -2583,8 +2867,16 @@
           <t>{'count': 30, 'unique': 1, 'top': True, 'freq': 30}</t>
         </is>
       </c>
-      <c r="H62" t="inlineStr"/>
-      <c r="I62" t="inlineStr"/>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>Booleano (True/False)</t>
+        </is>
+      </c>
       <c r="J62" t="inlineStr"/>
     </row>
     <row r="63">
@@ -2617,8 +2909,16 @@
           <t>{'count': 30, 'unique': 1, 'top': True, 'freq': 30}</t>
         </is>
       </c>
-      <c r="H63" t="inlineStr"/>
-      <c r="I63" t="inlineStr"/>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>Booleano (True/False)</t>
+        </is>
+      </c>
       <c r="J63" t="inlineStr"/>
     </row>
     <row r="64">
@@ -2651,8 +2951,16 @@
           <t>{'count': 30, 'unique': 2, 'top': False, 'freq': 25}</t>
         </is>
       </c>
-      <c r="H64" t="inlineStr"/>
-      <c r="I64" t="inlineStr"/>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>Booleano (True/False)</t>
+        </is>
+      </c>
       <c r="J64" t="inlineStr"/>
     </row>
     <row r="65">
@@ -2689,8 +2997,16 @@
           <t>{'count': 30.0, 'mean': 7945.8, 'std': 43334.536489008875, 'min': 0.0, '25%': 0.0, '50%': 2.0, '75%': 8.5, 'max': 237386.0}</t>
         </is>
       </c>
-      <c r="H65" t="inlineStr"/>
-      <c r="I65" t="inlineStr"/>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>ID codificado, entero positivo</t>
+        </is>
+      </c>
       <c r="J65" t="inlineStr"/>
     </row>
     <row r="66">
@@ -2723,7 +3039,11 @@
           <t>{'unique': 0, 'top': None, 'freq': None}</t>
         </is>
       </c>
-      <c r="H66" t="inlineStr"/>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I66" t="inlineStr"/>
       <c r="J66" t="inlineStr"/>
     </row>
@@ -2757,7 +3077,11 @@
           <t>{'count': 30, 'unique': 1, 'top': False, 'freq': 30}</t>
         </is>
       </c>
-      <c r="H67" t="inlineStr"/>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I67" t="inlineStr"/>
       <c r="J67" t="inlineStr"/>
     </row>
@@ -2791,7 +3115,11 @@
           <t>{'count': 30, 'unique': 1, 'top': False, 'freq': 30}</t>
         </is>
       </c>
-      <c r="H68" t="inlineStr"/>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I68" t="inlineStr"/>
       <c r="J68" t="inlineStr"/>
     </row>
@@ -2829,8 +3157,16 @@
           <t>{'count': 30.0, 'mean': 28.133333333333333, 'std': 150.5156042622717, 'min': 0.0, '25%': 0.0, '50%': 0.0, '75%': 0.0, 'max': 825.0}</t>
         </is>
       </c>
-      <c r="H69" t="inlineStr"/>
-      <c r="I69" t="inlineStr"/>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>ID codificado, entero positivo</t>
+        </is>
+      </c>
       <c r="J69" t="inlineStr"/>
     </row>
     <row r="70">
@@ -2863,7 +3199,11 @@
           <t>{'unique': 0, 'top': None, 'freq': None}</t>
         </is>
       </c>
-      <c r="H70" t="inlineStr"/>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I70" t="inlineStr"/>
       <c r="J70" t="inlineStr"/>
     </row>
@@ -2901,7 +3241,11 @@
           <t>{'count': 30.0, 'mean': 7945.8, 'std': 43334.536489008875, 'min': 0.0, '25%': 0.0, '50%': 2.0, '75%': 8.5, 'max': 237386.0}</t>
         </is>
       </c>
-      <c r="H71" t="inlineStr"/>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I71" t="inlineStr"/>
       <c r="J71" t="inlineStr"/>
     </row>
@@ -2939,7 +3283,11 @@
           <t>{'count': 30.0, 'mean': 28.133333333333333, 'std': 150.5156042622717, 'min': 0.0, '25%': 0.0, '50%': 0.0, '75%': 0.0, 'max': 825.0}</t>
         </is>
       </c>
-      <c r="H72" t="inlineStr"/>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I72" t="inlineStr"/>
       <c r="J72" t="inlineStr"/>
     </row>
@@ -2977,7 +3325,11 @@
           <t>{'count': 30.0, 'mean': 233.76666666666668, 'std': 1066.5860032359558, 'min': 0.0, '25%': 0.25, '50%': 3.5, '75%': 9.25, 'max': 5836.0}</t>
         </is>
       </c>
-      <c r="H73" t="inlineStr"/>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I73" t="inlineStr"/>
       <c r="J73" t="inlineStr"/>
     </row>
@@ -3011,7 +3363,11 @@
           <t>{'unique': 3, 'top': 'master', 'freq': 24}</t>
         </is>
       </c>
-      <c r="H74" t="inlineStr"/>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>https://api.github.com/</t>
+        </is>
+      </c>
       <c r="I74" t="inlineStr"/>
       <c r="J74" t="inlineStr"/>
     </row>

</xml_diff>